<commit_message>
Desacarga de matriz, Failed
</commit_message>
<xml_diff>
--- a/public/pages/admin/Matriz de hábilidades.xlsx
+++ b/public/pages/admin/Matriz de hábilidades.xlsx
@@ -15,24 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
-    <t>EJEMPLO PARA LA CELDA A1</t>
+    <t>Q5</t>
   </si>
   <si>
-    <t>EJEMPLO PARA LA CELDA B1</t>
-  </si>
-  <si>
-    <t>EJEMPLO PARA LA CELDA C1</t>
-  </si>
-  <si>
-    <t>EJEMPLO PARA LA CELDA D1</t>
-  </si>
-  <si>
-    <t>EJEMPLO PARA LA CELDA F1</t>
-  </si>
-  <si>
-    <t>EJEMPLO PARA LA CELDA G1</t>
+    <t>VORNE</t>
   </si>
 </sst>
 </file>
@@ -372,7 +360,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -380,24 +368,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>